<commit_message>
Checkin 4 27 2024
</commit_message>
<xml_diff>
--- a/SPRING -2024/8W2/ADTA 5340 - Discovery and Learning with Big Data/Assignment/4/Data Collection Second Round-Monte Littlejohn.xlsx
+++ b/SPRING -2024/8W2/ADTA 5340 - Discovery and Learning with Big Data/Assignment/4/Data Collection Second Round-Monte Littlejohn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Class\SPRING -2024\8W2\ADTA 5340 - Discovery and Learning with Big Data\Assignment\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E3EB66-59C8-4232-A5D0-94928A6FA718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BA7E45-DE2D-416F-AB4B-1AB1D5D8034E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="834" yWindow="-96" windowWidth="22302" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$N$63</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="142">
   <si>
     <t>COLLECTOR'S ID</t>
   </si>
@@ -59,9 +70,6 @@
   </si>
   <si>
     <t>COLLECTOR'S ANY OTHER RELEVANT NOTES OR LINKS</t>
-  </si>
-  <si>
-    <t>THE CONTENTS OF THE CELLS UNDER THESE COLUMNS SHOULD BE COMPLETED BY THE REVIEWER</t>
   </si>
   <si>
     <t>REVIEWER'S COARSE CATEGORY (POSITIVE, NEGATIVE OR NEUTRAL)</t>
@@ -862,9 +870,6 @@
     <t>https://www.naacpldf.org/wp-content/uploads/LDF_Bias_Report_WEB-2.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">There is studies stating that </t>
-  </si>
-  <si>
     <t>Colonialism is good for society</t>
   </si>
   <si>
@@ -874,19 +879,16 @@
     <t>BIASED</t>
   </si>
   <si>
-    <t>There is no benefit to colonialism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response is balanced and did not take any sides </t>
-  </si>
-  <si>
     <t xml:space="preserve">Balanced evidence was given </t>
   </si>
   <si>
     <t xml:space="preserve">Equal argement given </t>
   </si>
   <si>
-    <t xml:space="preserve">the repsonce is balanced and give right agrruemnt postive side of the arrgument </t>
+    <t>Use of technical language with NEUTRAL outcomes.</t>
+  </si>
+  <si>
+    <t>THE CONTENTS OF THE CELLS UNDER THESE COLUMNS SHOULD BE COMPLETED BY BINIAM ABEBE 11745787</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1425,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1433,13 +1435,13 @@
       <c r="E1" s="26"/>
       <c r="F1" s="27"/>
       <c r="G1" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
       <c r="J1" s="21"/>
       <c r="K1" s="22" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
@@ -1477,16 +1479,16 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -1494,33 +1496,33 @@
         <v>11605730</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="9">
         <v>45386.540972222225</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="17" t="s">
-        <v>125</v>
-      </c>
       <c r="N3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1528,33 +1530,33 @@
         <v>11605730</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9">
         <v>45386.552777777775</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
       <c r="K4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M4" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1562,33 +1564,33 @@
         <v>11605730</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
       <c r="K5" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M5" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" s="17" t="s">
         <v>128</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="244.8" x14ac:dyDescent="0.55000000000000004">
@@ -1596,30 +1598,30 @@
         <v>11605730</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="9">
         <v>45386.561111111114</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="12"/>
       <c r="K6" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -1627,33 +1629,33 @@
         <v>11605730</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="9">
         <v>45389.683333333334</v>
       </c>
       <c r="E7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
       <c r="K7" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
@@ -1661,27 +1663,30 @@
         <v>11605730</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="9">
         <v>45389.685416666667</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
       <c r="K8" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -1689,33 +1694,33 @@
         <v>11605730</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="9">
         <v>45389.6875</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
       <c r="K9" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L9" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M9" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -1723,27 +1728,30 @@
         <v>11605730</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="9">
         <v>45389.690972222219</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
       <c r="K10" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="216" x14ac:dyDescent="0.55000000000000004">
@@ -1751,27 +1759,30 @@
         <v>11605730</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="9">
         <v>45389.695138888892</v>
       </c>
       <c r="E11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
       <c r="K11" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -1779,27 +1790,30 @@
         <v>11605730</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="9">
         <v>45389.697222222225</v>
       </c>
       <c r="E12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="12"/>
       <c r="K12" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="16" t="s">
-        <v>124</v>
+      <c r="M12" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -1807,33 +1821,33 @@
         <v>11605730</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9">
         <v>45389.706250000003</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
       <c r="K13" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L13" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M13" s="17" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="244.8" x14ac:dyDescent="0.55000000000000004">
@@ -1841,32 +1855,32 @@
         <v>11605730</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="9">
         <v>45389.713888888888</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L14" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M14" s="17" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -1874,33 +1888,33 @@
         <v>11605730</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="9">
         <v>45389.715277777781</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
       <c r="K15" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M15" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="N15" s="17" t="s">
         <v>128</v>
-      </c>
-      <c r="N15" s="17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -1908,30 +1922,30 @@
         <v>11605730</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="9">
         <v>45389.716666666667</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="12"/>
       <c r="K16" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -1939,33 +1953,33 @@
         <v>11605730</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="9">
         <v>45389.717361111114</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
       <c r="K17" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M17" s="17" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -1973,27 +1987,30 @@
         <v>11605730</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="9">
         <v>45389.718055555553</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
       <c r="K18" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2001,33 +2018,33 @@
         <v>11605730</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="9">
         <v>45389.71875</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
       <c r="K19" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L19" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M19" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2035,27 +2052,30 @@
         <v>11605730</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="9">
         <v>45389.720138888886</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="12"/>
       <c r="K20" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2063,27 +2083,30 @@
         <v>11605730</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="9">
         <v>45389.720833333333</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
       <c r="K21" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2091,27 +2114,30 @@
         <v>11605730</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="9">
         <v>45389.72152777778</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
       <c r="K22" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L22" s="16" t="s">
-        <v>124</v>
+      <c r="M22" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2119,33 +2145,33 @@
         <v>11605730</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="9">
         <v>45389.723611111112</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
       <c r="K23" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L23" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M23" s="17" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N23" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2153,33 +2179,33 @@
         <v>11605730</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="9">
         <v>45389.725694444445</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
       <c r="K24" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M24" s="17" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="N24" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2187,33 +2213,33 @@
         <v>11605730</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="9">
         <v>45389.726388888892</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
       <c r="K25" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M25" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="N25" s="17" t="s">
         <v>128</v>
-      </c>
-      <c r="N25" s="17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2221,30 +2247,30 @@
         <v>11605730</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="9">
         <v>45389.725694444445</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="12"/>
       <c r="K26" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2252,33 +2278,33 @@
         <v>11605730</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="9">
         <v>45389.729166666664</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="12"/>
       <c r="K27" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L27" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M27" s="17" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -2286,27 +2312,30 @@
         <v>11605730</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="9">
         <v>45389.730555555558</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="12"/>
       <c r="K28" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2314,33 +2343,33 @@
         <v>11605730</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="9">
         <v>45389.731944444444</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
       <c r="K29" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L29" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M29" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2348,27 +2377,30 @@
         <v>11605730</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="9">
         <v>45389.73333333333</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="11"/>
       <c r="J30" s="12"/>
       <c r="K30" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2376,26 +2408,29 @@
         <v>11605730</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="9">
         <v>45389.734027777777</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I31" s="11"/>
       <c r="K31" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2403,26 +2438,29 @@
         <v>11605730</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="9">
         <v>45389.73541666667</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I32" s="11"/>
       <c r="K32" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L32" s="16" t="s">
-        <v>124</v>
+      <c r="M32" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="388.8" x14ac:dyDescent="0.55000000000000004">
@@ -2430,26 +2468,26 @@
         <v>11605730</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I33" s="11"/>
       <c r="K33" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M33" s="17" t="s">
         <v>140</v>
@@ -2460,29 +2498,29 @@
         <v>11605730</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="I34" s="11"/>
       <c r="K34" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L34" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M34" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="374.4" x14ac:dyDescent="0.55000000000000004">
@@ -2490,26 +2528,29 @@
         <v>11605730</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E35" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="I35" s="11"/>
       <c r="K35" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L35" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L35" s="16" t="s">
-        <v>124</v>
+      <c r="M35" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="360" x14ac:dyDescent="0.55000000000000004">
@@ -2517,26 +2558,29 @@
         <v>11605730</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E36" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="I36" s="11"/>
       <c r="K36" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="374.4" x14ac:dyDescent="0.55000000000000004">
@@ -2544,26 +2588,29 @@
         <v>11605730</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E37" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="I37" s="11"/>
       <c r="K37" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="374.4" x14ac:dyDescent="0.55000000000000004">
@@ -2571,26 +2618,29 @@
         <v>11605730</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E38" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="I38" s="11"/>
       <c r="K38" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2598,26 +2648,29 @@
         <v>11605730</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E39" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="I39" s="11"/>
       <c r="K39" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2625,26 +2678,29 @@
         <v>11605730</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E40" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="I40" s="11"/>
       <c r="K40" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2652,26 +2708,29 @@
         <v>11605730</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E41" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="I41" s="11"/>
       <c r="K41" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2679,26 +2738,29 @@
         <v>11605730</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E42" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="I42" s="11"/>
       <c r="K42" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2706,26 +2768,29 @@
         <v>11605730</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E43" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="I43" s="11"/>
       <c r="K43" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L43" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2733,26 +2798,29 @@
         <v>11605730</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E44" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="I44" s="11"/>
       <c r="K44" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L44" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2760,26 +2828,29 @@
         <v>11605730</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E45" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="I45" s="11"/>
       <c r="K45" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L45" s="16" t="s">
-        <v>124</v>
+      <c r="M45" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2787,29 +2858,29 @@
         <v>11605730</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="I46" s="11"/>
       <c r="K46" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L46" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="M46" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2817,29 +2888,29 @@
         <v>11605730</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="I47" s="11"/>
       <c r="K47" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M47" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2847,26 +2918,29 @@
         <v>11605730</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E48" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="I48" s="11"/>
       <c r="K48" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L48" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M48" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2874,29 +2948,29 @@
         <v>11605730</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E49" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="I49" s="11"/>
       <c r="K49" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L49" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M49" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2904,26 +2978,29 @@
         <v>11605730</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E50" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F50" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>96</v>
       </c>
       <c r="I50" s="11"/>
       <c r="K50" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L50" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M50" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2931,26 +3008,29 @@
         <v>11605730</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>98</v>
       </c>
       <c r="I51" s="11"/>
       <c r="K51" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L51" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M51" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2958,26 +3038,29 @@
         <v>11605730</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="I52" s="11"/>
       <c r="K52" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L52" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M52" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -2985,26 +3068,29 @@
         <v>11605730</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E53" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>102</v>
       </c>
       <c r="I53" s="11"/>
       <c r="K53" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L53" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3012,26 +3098,29 @@
         <v>11605730</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E54" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>104</v>
       </c>
       <c r="I54" s="11"/>
       <c r="K54" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3039,26 +3128,29 @@
         <v>11605730</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E55" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="I55" s="11"/>
       <c r="K55" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L55" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M55" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3066,26 +3158,29 @@
         <v>11605730</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E56" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>108</v>
       </c>
       <c r="I56" s="11"/>
       <c r="K56" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L56" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M56" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3093,26 +3188,29 @@
         <v>11605730</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E57" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="I57" s="11"/>
       <c r="K57" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L57" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3120,26 +3218,29 @@
         <v>11605730</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E58" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="I58" s="11"/>
       <c r="K58" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L58" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3147,26 +3248,29 @@
         <v>11605730</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E59" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="I59" s="11"/>
       <c r="K59" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L59" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3174,26 +3278,29 @@
         <v>11605730</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E60" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="I60" s="11"/>
       <c r="K60" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3201,26 +3308,29 @@
         <v>11605730</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E61" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" s="10" t="s">
         <v>117</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>118</v>
       </c>
       <c r="I61" s="11"/>
       <c r="K61" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L61" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3228,26 +3338,29 @@
         <v>11605730</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E62" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="I62" s="11"/>
       <c r="K62" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L62" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M62" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3255,29 +3368,33 @@
         <v>11605730</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" s="9">
         <v>45393.854166666664</v>
       </c>
       <c r="E63" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>122</v>
       </c>
       <c r="I63" s="11"/>
       <c r="K63" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L63" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="M63" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:N63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>

</xml_diff>